<commit_message>
changed so that we receive the form data in the frontmatter of the setup.astro page and handle the excel processing there, then on the formsubmit it re-renders the page so the data is passed to the SetupColumn component
</commit_message>
<xml_diff>
--- a/public/Book1.xlsx
+++ b/public/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zach/Documents/Dev/bby-htmx/portal/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE481C93-28E6-8348-B02E-A6A26EFFB9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07FEB6A-466E-C64C-B2CE-9A6FD2809E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{CDD4735F-1E1F-1C43-9035-C44897980F9A}"/>
+    <workbookView xWindow="2200" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{CDD4735F-1E1F-1C43-9035-C44897980F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>SKU</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>BIG SMALL TING</t>
+  </si>
+  <si>
+    <t>SMALL LITTLE BIG TING</t>
+  </si>
+  <si>
+    <t>WHAT</t>
   </si>
 </sst>
 </file>
@@ -422,13 +428,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310246DC-1A36-AC46-8DCF-849BB00C2A43}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -450,6 +461,17 @@
       </c>
       <c r="C2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20202020</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed when user uploads nothing it crashes the site
</commit_message>
<xml_diff>
--- a/public/Book1.xlsx
+++ b/public/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zach/Documents/Dev/bby-htmx/portal/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07FEB6A-466E-C64C-B2CE-9A6FD2809E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EF0713-C113-D94E-8A2A-5EADB7FC8B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{CDD4735F-1E1F-1C43-9035-C44897980F9A}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>SKU</t>
-  </si>
-  <si>
     <t>SKU_DESC</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>WHAT</t>
+  </si>
+  <si>
+    <t>VPN</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,13 +443,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -457,10 +457,10 @@
         <v>10101010</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -468,10 +468,10 @@
         <v>20202020</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added spinner component to show user uploading
</commit_message>
<xml_diff>
--- a/public/Book1.xlsx
+++ b/public/Book1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zach/Documents/Dev/bby-htmx/portal/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EF0713-C113-D94E-8A2A-5EADB7FC8B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E611B4-9E5A-A44D-899E-CB627A76DDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{CDD4735F-1E1F-1C43-9035-C44897980F9A}"/>
+    <workbookView xWindow="39300" yWindow="1220" windowWidth="38400" windowHeight="21100" xr2:uid="{CDD4735F-1E1F-1C43-9035-C44897980F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>SKU_DESC</t>
   </si>
@@ -57,6 +57,36 @@
   </si>
   <si>
     <t>VPN</t>
+  </si>
+  <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>SECONDARY_UPC</t>
+  </si>
+  <si>
+    <t>BRAND_NAME</t>
+  </si>
+  <si>
+    <t>MODEL_NO</t>
+  </si>
+  <si>
+    <t>MANUFACTURER</t>
+  </si>
+  <si>
+    <t>UNIT_COST</t>
+  </si>
+  <si>
+    <t>ORIGINAL_RETAIL</t>
+  </si>
+  <si>
+    <t>Alfalfa</t>
+  </si>
+  <si>
+    <t>Asus</t>
+  </si>
+  <si>
+    <t>ENT_STREET_DATE</t>
   </si>
 </sst>
 </file>
@@ -92,8 +122,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,50 +459,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310246DC-1A36-AC46-8DCF-849BB00C2A43}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10101010</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="D2">
+        <v>12345678910</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>1032423</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>1.26</v>
+      </c>
+      <c r="J2">
+        <v>2.89</v>
+      </c>
+      <c r="K2" s="1">
+        <v>44677</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20202020</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="D3">
+        <v>12345678912</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>1032423</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>1.26</v>
+      </c>
+      <c r="J3">
+        <v>2.89</v>
+      </c>
+      <c r="K3" s="1">
+        <v>45443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new compliancecolumn component as there were too many differences
</commit_message>
<xml_diff>
--- a/public/Book1.xlsx
+++ b/public/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zach/Documents/Dev/bby-htmx/portal/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E611B4-9E5A-A44D-899E-CB627A76DDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64ECC10-7D9B-2048-A0BC-DCA5E280C448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39300" yWindow="1220" windowWidth="38400" windowHeight="21100" xr2:uid="{CDD4735F-1E1F-1C43-9035-C44897980F9A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CDD4735F-1E1F-1C43-9035-C44897980F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>SKU_DESC</t>
   </si>
@@ -87,6 +87,45 @@
   </si>
   <si>
     <t>ENT_STREET_DATE</t>
+  </si>
+  <si>
+    <t>SHIP_CARTON_WID</t>
+  </si>
+  <si>
+    <t>SHIP_CARTON_LEN</t>
+  </si>
+  <si>
+    <t>SHIP_CARTON_HT</t>
+  </si>
+  <si>
+    <t>SHIP_CARTON_WT</t>
+  </si>
+  <si>
+    <t>S_UNIT_WIDTH</t>
+  </si>
+  <si>
+    <t>S_UNIT_HEIGHT</t>
+  </si>
+  <si>
+    <t>S_UNIT_LENGTH</t>
+  </si>
+  <si>
+    <t>S_UNIT_WEIGHT</t>
+  </si>
+  <si>
+    <t>SUPP_PACK_SIZE</t>
+  </si>
+  <si>
+    <t>INNERPACK_SIZE</t>
+  </si>
+  <si>
+    <t>FRENCH_COMPLIANT</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -459,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310246DC-1A36-AC46-8DCF-849BB00C2A43}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,9 +515,14 @@
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -512,8 +556,41 @@
       <c r="K1" t="s">
         <v>16</v>
       </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10101010</v>
       </c>
@@ -544,8 +621,41 @@
       <c r="K2" s="1">
         <v>44677</v>
       </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20202020</v>
       </c>
@@ -575,6 +685,39 @@
       </c>
       <c r="K3" s="1">
         <v>45443</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>